<commit_message>
Save work before switching to main
</commit_message>
<xml_diff>
--- a/Data/PoerBIdata.xlsx
+++ b/Data/PoerBIdata.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Personal_Projects\Covid_Parcel_Business_Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{81F3B3FB-2E90-493E-B38A-C630D515EAB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0161BD26-7C0C-4C19-8405-5BEFCB00EBB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{583C2690-A594-41DF-B266-133638D4CB7F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{583C2690-A594-41DF-B266-133638D4CB7F}"/>
   </bookViews>
   <sheets>
     <sheet name="lost" sheetId="1" r:id="rId1"/>
     <sheet name="New" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t>Customer_Group_2019</t>
   </si>
@@ -87,13 +88,38 @@
   </si>
   <si>
     <t>Revenue_%Change</t>
+  </si>
+  <si>
+    <t>Growth_Category</t>
+  </si>
+  <si>
+    <t>Declining Customers</t>
+  </si>
+  <si>
+    <t>High Growth Customers</t>
+  </si>
+  <si>
+    <t>Lost Customers</t>
+  </si>
+  <si>
+    <t>Stable Customers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,23 +164,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="11" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -538,7 +571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA973A88-F79A-48E7-A5A9-7A1EB9C7E2DA}">
   <dimension ref="B1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A6"/>
     </sheetView>
   </sheetViews>
@@ -619,7 +652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F07E9F-0E7E-494D-8F47-80AE716FE69E}">
   <dimension ref="B1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A6"/>
     </sheetView>
   </sheetViews>
@@ -766,4 +799,190 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{212CDA01-B5BA-4289-9972-23769B0AAF31}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>44</v>
+      </c>
+      <c r="C5" s="2">
+        <v>171</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2">
+        <v>84</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>11</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f>SUM(B6:E6)</f>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>241</v>
+      </c>
+      <c r="C7" s="2">
+        <v>386</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>54</v>
+      </c>
+      <c r="F7">
+        <f>SUM(B7:E7)</f>
+        <v>681</v>
+      </c>
+      <c r="G7" s="5">
+        <f>B6+B7</f>
+        <v>325</v>
+      </c>
+      <c r="H7">
+        <f>F7+F6</f>
+        <v>776</v>
+      </c>
+      <c r="I7" s="6">
+        <f>G7/H7</f>
+        <v>0.41881443298969073</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B8">
+        <f>SUM(B2:B7)</f>
+        <v>373</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:E8" si="0">SUM(C2:C7)</f>
+        <v>586</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="F8">
+        <f>SUM(B8:E8)</f>
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B9" s="4">
+        <f>B8/$F$8</f>
+        <v>0.35659655831739961</v>
+      </c>
+      <c r="C9" s="4">
+        <f t="shared" ref="C9:E9" si="1">C8/$F$8</f>
+        <v>0.56022944550669218</v>
+      </c>
+      <c r="D9" s="4">
+        <f t="shared" si="1"/>
+        <v>1.0516252390057362E-2</v>
+      </c>
+      <c r="E9" s="4">
+        <f t="shared" si="1"/>
+        <v>7.2657743785850867E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>